<commit_message>
[update] add more data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hkt\mvp\data_populator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hkt\mvp\data_populator\argo-ai-data-populator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA0E11D-62DA-44A3-8EF3-EA5C0317A90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0A8A72-0FEF-40F4-8ED3-2297BD9704FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>